<commit_message>
EPBDS-10234 Fix bug with tests
</commit_message>
<xml_diff>
--- a/DEMO/org.openl.rules.demo/data/openl-demo/design-repository/DESIGN/rules/Tutorial 8 - Introduction to Smart Rules and Smart Lookup Tables/Tutorial8 - Introduction to Smart Rules and Smart Lookup Tables.xlsx
+++ b/DEMO/org.openl.rules.demo/data/openl-demo/design-repository/DESIGN/rules/Tutorial 8 - Introduction to Smart Rules and Smart Lookup Tables/Tutorial8 - Introduction to Smart Rules and Smart Lookup Tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsimanenka\Downloads\"/>
     </mc:Choice>
@@ -1889,7 +1889,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -1945,13 +1945,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" rgb="FFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1975,7 +1975,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2130,15 +2130,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="1">
+  <cellStyleXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="44" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="4"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2231,16 +2233,16 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2258,10 +2260,10 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2282,13 +2284,13 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="8" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="8" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2296,10 +2298,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2309,10 +2311,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2336,7 +2338,7 @@
     <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2426,16 +2428,16 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2505,12 +2507,14 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
+    <cellStyle name="Currency" xfId="6" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{512ECBAB-01CC-4947-A4D6-AE892C1C0EEC}"/>
-    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{512ECBAB-01CC-4947-A4D6-AE892C1C0EEC}"/>
+    <cellStyle name="Normal 6" xfId="5" xr:uid="{C13E7B46-80D0-47AB-ABD3-ED1A9145A7FB}"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Обычный 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4982,11 +4986,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" style="2" width="9.109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="2" width="13.109375" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="2" width="10.5546875" collapsed="false"/>
-    <col min="10" max="11" customWidth="true" style="2" width="9.109375" collapsed="false"/>
-    <col min="12" max="16384" style="2" width="9.109375" collapsed="false"/>
+    <col min="1" max="7" width="9.109375" style="2"/>
+    <col min="8" max="8" width="13.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5336,14 +5340,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="8.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="4" width="12.33203125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="28.77734375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="42.109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="4" width="17.33203125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="28.77734375" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="4" width="9.109375" collapsed="false"/>
-    <col min="8" max="16384" style="4" width="8.88671875" collapsed="false"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="12.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -6093,16 +6097,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="8.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="4" width="12.33203125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="21.109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="12.21875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="21.33203125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="5.21875" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="22.6640625" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="4.5546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="4" width="9.109375" collapsed="false"/>
-    <col min="10" max="16384" style="4" width="8.88671875" collapsed="false"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="12.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -6881,14 +6885,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="8.88671875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="4" width="5.5546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="4" width="28.44140625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="4" width="27.88671875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="10.6640625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="42.109375" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="4" width="5.44140625" collapsed="false"/>
-    <col min="8" max="16384" style="4" width="8.88671875" collapsed="false"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="5.5546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -7625,16 +7629,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="4" width="8.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="4" width="43.21875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="4" width="45.88671875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="4" width="27.88671875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="31.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="18.77734375" collapsed="false"/>
-    <col min="8" max="8" style="4" width="8.88671875" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="6.6640625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="4" width="18.77734375" collapsed="false"/>
-    <col min="11" max="16384" style="4" width="8.88671875" collapsed="false"/>
+    <col min="1" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="43.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -8852,13 +8856,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="4" width="8.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="4" width="18.5546875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="55.44140625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="23.21875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="4" width="26.6640625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="4" width="17.109375" collapsed="false"/>
-    <col min="8" max="16384" style="4" width="8.88671875" collapsed="false"/>
+    <col min="1" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="18.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="19.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -9156,8 +9160,8 @@
         <v>135</v>
       </c>
       <c r="D34" s="83"/>
-      <c r="E34" s="59" t="n">
-        <v>0.81</v>
+      <c r="E34" s="59">
+        <v>0.8</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>

</xml_diff>